<commit_message>
Update ACCESS Variable Dictionary 2018-2019.xlsx
</commit_message>
<xml_diff>
--- a/ACCESS Variable Dictionary 2018-2019.xlsx
+++ b/ACCESS Variable Dictionary 2018-2019.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="175">
   <si>
     <t>Variable</t>
   </si>
@@ -323,18 +323,6 @@
     <t>ACCESS</t>
   </si>
   <si>
-    <t>cbt_listen</t>
-  </si>
-  <si>
-    <t>cbt_read</t>
-  </si>
-  <si>
-    <t>cbt_speak</t>
-  </si>
-  <si>
-    <t>cbt_write</t>
-  </si>
-  <si>
     <t>2 levels: Online, Paper</t>
   </si>
   <si>
@@ -504,6 +492,63 @@
   </si>
   <si>
     <t>2 levels: Plan 504, not Plan 504</t>
+  </si>
+  <si>
+    <t>mode_listen</t>
+  </si>
+  <si>
+    <t>mode_read</t>
+  </si>
+  <si>
+    <t>mode_speak</t>
+  </si>
+  <si>
+    <t>mode_write</t>
+  </si>
+  <si>
+    <t>missing_listen</t>
+  </si>
+  <si>
+    <t>missing_read</t>
+  </si>
+  <si>
+    <t>missing_speak</t>
+  </si>
+  <si>
+    <t>missing_write</t>
+  </si>
+  <si>
+    <t>missing_domains</t>
+  </si>
+  <si>
+    <t>whether the listening score is missing</t>
+  </si>
+  <si>
+    <t>whether the reading score is missing</t>
+  </si>
+  <si>
+    <t>whether the speaking score is missing</t>
+  </si>
+  <si>
+    <t>whether the writeing score is missing</t>
+  </si>
+  <si>
+    <t>2 levels: 1 = missing, 0 = not missing</t>
+  </si>
+  <si>
+    <t>number of domains that have missing scores</t>
+  </si>
+  <si>
+    <t>0-4</t>
+  </si>
+  <si>
+    <t>3 levels: 1 = missing, 0 = not missing</t>
+  </si>
+  <si>
+    <t>4 levels: 1 = missing, 0 = not missing</t>
+  </si>
+  <si>
+    <t>5 levels: 1 = missing, 0 = not missing</t>
   </si>
 </sst>
 </file>
@@ -568,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -596,6 +641,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,10 +928,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,17 +1355,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G21" s="7"/>
     </row>
@@ -1516,7 +1564,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
@@ -1526,7 +1574,7 @@
         <v>68</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G32" s="7"/>
     </row>
@@ -1535,7 +1583,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
@@ -1545,7 +1593,7 @@
         <v>68</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G33" s="7"/>
     </row>
@@ -1554,7 +1602,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
@@ -1564,7 +1612,7 @@
         <v>68</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G34" s="7"/>
     </row>
@@ -1573,7 +1621,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
@@ -1583,7 +1631,7 @@
         <v>68</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G35" s="7"/>
     </row>
@@ -1599,7 +1647,7 @@
         <v>53</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="7"/>
@@ -1609,17 +1657,17 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G37" s="7"/>
     </row>
@@ -1628,17 +1676,17 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G38" s="7"/>
     </row>
@@ -1647,17 +1695,17 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G39" s="7"/>
     </row>
@@ -1666,17 +1714,17 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G40" s="7"/>
     </row>
@@ -1685,20 +1733,20 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1706,20 +1754,20 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1727,20 +1775,20 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1748,20 +1796,20 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1769,17 +1817,17 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G45" s="7"/>
     </row>
@@ -1788,17 +1836,17 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G46" s="7"/>
     </row>
@@ -1807,17 +1855,17 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G47" s="7"/>
     </row>
@@ -1826,17 +1874,17 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G48" s="7"/>
     </row>
@@ -1845,17 +1893,17 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G49" s="7"/>
     </row>
@@ -1864,17 +1912,17 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G50" s="7"/>
     </row>
@@ -1883,17 +1931,17 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G51" s="7"/>
     </row>
@@ -1902,17 +1950,17 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G52" s="7"/>
     </row>
@@ -1938,20 +1986,20 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1959,20 +2007,20 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1980,20 +2028,20 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E56" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G56" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2001,20 +2049,20 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2032,9 +2080,104 @@
         <v>69</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="10"/>
+      <c r="D60" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" s="10"/>
+      <c r="D61" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" s="10"/>
+      <c r="D62" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>62</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C63" s="10"/>
+      <c r="D63" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="G63" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>